<commit_message>
Arreglar nombres de columnas
</commit_message>
<xml_diff>
--- a/Datos/Energia/Corredor Energia.xlsx
+++ b/Datos/Energia/Corredor Energia.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27214"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Quique/Documents/Corredor Interoceanico/1. Documentos de Respaldo/2. Corredor Interoceánico/Negocios de Transporte/Factibilidad/Actualización/analisis-financiero/Datos/Energia/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saulmendezaguirre/Documents/Axon/Analis financiero CIG/analisis-financiero/Datos/Energia/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5820" yWindow="2940" windowWidth="28800" windowHeight="17600" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Inversiones" sheetId="1" r:id="rId1"/>
     <sheet name="Costos" sheetId="2" r:id="rId2"/>
     <sheet name="Ingresos" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000" iterate="1" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="17">
   <si>
     <t>Mantenimiento</t>
   </si>
@@ -73,16 +73,13 @@
     <t>Fase 1</t>
   </si>
   <si>
-    <t>Categoría</t>
-  </si>
-  <si>
-    <t>Costos.Operación</t>
-  </si>
-  <si>
     <t>Ingresos.Operación</t>
   </si>
   <si>
     <t>Explotacion</t>
+  </si>
+  <si>
+    <t>Costos.Operacion</t>
   </si>
 </sst>
 </file>
@@ -118,9 +115,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,376 +396,379 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DI5"/>
+  <dimension ref="A1:DJ5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="44.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="44.33203125" customWidth="1"/>
-    <col min="5" max="13" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="44.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="44.33203125" customWidth="1"/>
+    <col min="6" max="14" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:113" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:114" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" t="s">
-        <v>14</v>
-      </c>
       <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
         <v>12</v>
       </c>
-      <c r="E1">
+      <c r="F1">
         <v>2012</v>
       </c>
-      <c r="F1">
+      <c r="G1">
         <v>2013</v>
       </c>
-      <c r="G1">
+      <c r="H1">
         <v>2014</v>
       </c>
-      <c r="H1">
+      <c r="I1">
         <v>2015</v>
       </c>
-      <c r="I1">
+      <c r="J1">
         <v>2016</v>
       </c>
-      <c r="J1">
+      <c r="K1">
         <v>2017</v>
       </c>
-      <c r="K1">
+      <c r="L1">
         <v>2018</v>
       </c>
-      <c r="L1">
+      <c r="M1">
         <v>2019</v>
       </c>
-      <c r="M1">
+      <c r="N1">
         <v>2020</v>
       </c>
-      <c r="N1">
+      <c r="O1">
         <v>2021</v>
       </c>
-      <c r="O1">
+      <c r="P1">
         <v>2022</v>
       </c>
-      <c r="P1">
+      <c r="Q1">
         <v>2023</v>
       </c>
-      <c r="Q1">
+      <c r="R1">
         <v>2024</v>
       </c>
-      <c r="R1">
+      <c r="S1">
         <v>2025</v>
       </c>
-      <c r="S1">
+      <c r="T1">
         <v>2026</v>
       </c>
-      <c r="T1">
+      <c r="U1">
         <v>2027</v>
       </c>
-      <c r="U1">
+      <c r="V1">
         <v>2028</v>
       </c>
-      <c r="V1">
+      <c r="W1">
         <v>2029</v>
       </c>
-      <c r="W1">
+      <c r="X1">
         <v>2030</v>
       </c>
-      <c r="X1">
+      <c r="Y1">
         <v>2031</v>
       </c>
-      <c r="Y1">
+      <c r="Z1">
         <v>2032</v>
       </c>
-      <c r="Z1">
+      <c r="AA1">
         <v>2033</v>
       </c>
-      <c r="AA1">
+      <c r="AB1">
         <v>2034</v>
       </c>
-      <c r="AB1">
+      <c r="AC1">
         <v>2035</v>
       </c>
-      <c r="AC1">
+      <c r="AD1">
         <v>2036</v>
       </c>
-      <c r="AD1">
+      <c r="AE1">
         <v>2037</v>
       </c>
-      <c r="AE1">
+      <c r="AF1">
         <v>2038</v>
       </c>
-      <c r="AF1">
+      <c r="AG1">
         <v>2039</v>
       </c>
-      <c r="AG1">
+      <c r="AH1">
         <v>2040</v>
       </c>
-      <c r="AH1">
+      <c r="AI1">
         <v>2041</v>
       </c>
-      <c r="AI1">
+      <c r="AJ1">
         <v>2042</v>
       </c>
-      <c r="AJ1">
+      <c r="AK1">
         <v>2043</v>
       </c>
-      <c r="AK1">
+      <c r="AL1">
         <v>2044</v>
       </c>
-      <c r="AL1">
+      <c r="AM1">
         <v>2045</v>
       </c>
-      <c r="AM1">
+      <c r="AN1">
         <v>2046</v>
       </c>
-      <c r="AN1">
+      <c r="AO1">
         <v>2047</v>
       </c>
-      <c r="AO1">
+      <c r="AP1">
         <v>2048</v>
       </c>
-      <c r="AP1">
+      <c r="AQ1">
         <v>2049</v>
       </c>
-      <c r="AQ1">
+      <c r="AR1">
         <v>2050</v>
       </c>
-      <c r="AR1">
+      <c r="AS1">
         <v>2051</v>
       </c>
-      <c r="AS1">
+      <c r="AT1">
         <v>2052</v>
       </c>
-      <c r="AT1">
+      <c r="AU1">
         <v>2053</v>
       </c>
-      <c r="AU1">
+      <c r="AV1">
         <v>2054</v>
       </c>
-      <c r="AV1">
+      <c r="AW1">
         <v>2055</v>
       </c>
-      <c r="AW1">
+      <c r="AX1">
         <v>2056</v>
       </c>
-      <c r="AX1">
+      <c r="AY1">
         <v>2057</v>
       </c>
-      <c r="AY1">
+      <c r="AZ1">
         <v>2058</v>
       </c>
-      <c r="AZ1">
+      <c r="BA1">
         <v>2059</v>
       </c>
-      <c r="BA1">
+      <c r="BB1">
         <v>2060</v>
       </c>
-      <c r="BB1">
+      <c r="BC1">
         <v>2061</v>
       </c>
-      <c r="BC1">
+      <c r="BD1">
         <v>2062</v>
       </c>
-      <c r="BD1">
+      <c r="BE1">
         <v>2063</v>
       </c>
-      <c r="BE1">
+      <c r="BF1">
         <v>2064</v>
       </c>
-      <c r="BF1">
+      <c r="BG1">
         <v>2065</v>
       </c>
-      <c r="BG1">
+      <c r="BH1">
         <v>2066</v>
       </c>
-      <c r="BH1">
+      <c r="BI1">
         <v>2067</v>
       </c>
-      <c r="BI1">
+      <c r="BJ1">
         <v>2068</v>
       </c>
-      <c r="BJ1">
+      <c r="BK1">
         <v>2069</v>
       </c>
-      <c r="BK1">
+      <c r="BL1">
         <v>2070</v>
       </c>
-      <c r="BL1">
+      <c r="BM1">
         <v>2071</v>
       </c>
-      <c r="BM1">
+      <c r="BN1">
         <v>2072</v>
       </c>
-      <c r="BN1">
+      <c r="BO1">
         <v>2073</v>
       </c>
-      <c r="BO1">
+      <c r="BP1">
         <v>2074</v>
       </c>
-      <c r="BP1">
+      <c r="BQ1">
         <v>2075</v>
       </c>
-      <c r="BQ1">
+      <c r="BR1">
         <v>2076</v>
       </c>
-      <c r="BR1">
+      <c r="BS1">
         <v>2077</v>
       </c>
-      <c r="BS1">
+      <c r="BT1">
         <v>2078</v>
       </c>
-      <c r="BT1">
+      <c r="BU1">
         <v>2079</v>
       </c>
-      <c r="BU1">
+      <c r="BV1">
         <v>2080</v>
       </c>
-      <c r="BV1">
+      <c r="BW1">
         <v>2081</v>
       </c>
-      <c r="BW1">
+      <c r="BX1">
         <v>2082</v>
       </c>
-      <c r="BX1">
+      <c r="BY1">
         <v>2083</v>
       </c>
-      <c r="BY1">
+      <c r="BZ1">
         <v>2084</v>
       </c>
-      <c r="BZ1">
+      <c r="CA1">
         <v>2085</v>
       </c>
-      <c r="CA1">
+      <c r="CB1">
         <v>2086</v>
       </c>
-      <c r="CB1">
+      <c r="CC1">
         <v>2087</v>
       </c>
-      <c r="CC1">
+      <c r="CD1">
         <v>2088</v>
       </c>
-      <c r="CD1">
+      <c r="CE1">
         <v>2089</v>
       </c>
-      <c r="CE1">
+      <c r="CF1">
         <v>2090</v>
       </c>
-      <c r="CF1">
+      <c r="CG1">
         <v>2091</v>
       </c>
-      <c r="CG1">
+      <c r="CH1">
         <v>2092</v>
       </c>
-      <c r="CH1">
+      <c r="CI1">
         <v>2093</v>
       </c>
-      <c r="CI1">
+      <c r="CJ1">
         <v>2094</v>
       </c>
-      <c r="CJ1">
+      <c r="CK1">
         <v>2095</v>
       </c>
-      <c r="CK1">
+      <c r="CL1">
         <v>2096</v>
       </c>
-      <c r="CL1">
+      <c r="CM1">
         <v>2097</v>
       </c>
-      <c r="CM1">
+      <c r="CN1">
         <v>2098</v>
       </c>
-      <c r="CN1">
+      <c r="CO1">
         <v>2099</v>
       </c>
-      <c r="CO1">
+      <c r="CP1">
         <v>2100</v>
       </c>
-      <c r="CP1">
+      <c r="CQ1">
         <v>2101</v>
       </c>
-      <c r="CQ1">
+      <c r="CR1">
         <v>2102</v>
       </c>
-      <c r="CR1">
+      <c r="CS1">
         <v>2103</v>
       </c>
-      <c r="CS1">
+      <c r="CT1">
         <v>2104</v>
       </c>
-      <c r="CT1">
+      <c r="CU1">
         <v>2105</v>
       </c>
-      <c r="CU1">
+      <c r="CV1">
         <v>2106</v>
       </c>
-      <c r="CV1">
+      <c r="CW1">
         <v>2107</v>
       </c>
-      <c r="CW1">
+      <c r="CX1">
         <v>2108</v>
       </c>
-      <c r="CX1">
+      <c r="CY1">
         <v>2109</v>
       </c>
-      <c r="CY1">
+      <c r="CZ1">
         <v>2110</v>
       </c>
-      <c r="CZ1">
+      <c r="DA1">
         <v>2111</v>
       </c>
-      <c r="DA1">
+      <c r="DB1">
         <v>2112</v>
       </c>
-      <c r="DB1">
+      <c r="DC1">
         <v>2113</v>
       </c>
-      <c r="DC1">
+      <c r="DD1">
         <v>2114</v>
       </c>
-      <c r="DD1">
+      <c r="DE1">
         <v>2115</v>
       </c>
-      <c r="DE1">
+      <c r="DF1">
         <v>2116</v>
       </c>
-      <c r="DF1">
+      <c r="DG1">
         <v>2117</v>
       </c>
-      <c r="DG1">
+      <c r="DH1">
         <v>2118</v>
       </c>
-      <c r="DH1">
+      <c r="DI1">
         <v>2119</v>
       </c>
-      <c r="DI1">
+      <c r="DJ1">
         <v>2120</v>
       </c>
     </row>
-    <row r="2" spans="1:113" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:114" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>13</v>
       </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
       <c r="F2">
         <v>0</v>
       </c>
@@ -775,17 +776,17 @@
         <v>0</v>
       </c>
       <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
         <v>69401</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>71136</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>72914</v>
       </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
       <c r="L2">
         <v>0</v>
       </c>
@@ -1092,23 +1093,26 @@
       <c r="DI2">
         <v>0</v>
       </c>
+      <c r="DJ2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:113" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:114" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>13</v>
       </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
       <c r="F3">
         <v>0</v>
       </c>
@@ -1116,17 +1120,17 @@
         <v>0</v>
       </c>
       <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
         <v>112955</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>115779</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>118673</v>
       </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
       <c r="L3">
         <v>0</v>
       </c>
@@ -1433,23 +1437,26 @@
       <c r="DI3">
         <v>0</v>
       </c>
+      <c r="DJ3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:113" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:114" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>13</v>
       </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
       <c r="F4">
         <v>0</v>
       </c>
@@ -1457,17 +1464,17 @@
         <v>0</v>
       </c>
       <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
         <v>832724</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>853542</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>874880</v>
       </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
       <c r="L4">
         <v>0</v>
       </c>
@@ -1774,23 +1781,26 @@
       <c r="DI4">
         <v>0</v>
       </c>
+      <c r="DJ4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:113" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:114" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>13</v>
       </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
       <c r="F5">
         <v>0</v>
       </c>
@@ -1798,17 +1808,17 @@
         <v>0</v>
       </c>
       <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
         <v>141791</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>145335</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>148969</v>
       </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
       <c r="L5">
         <v>0</v>
       </c>
@@ -2113,6 +2123,9 @@
         <v>0</v>
       </c>
       <c r="DI5">
+        <v>0</v>
+      </c>
+      <c r="DJ5">
         <v>0</v>
       </c>
     </row>
@@ -2125,8 +2138,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DI4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2141,7 +2154,7 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
         <v>8</v>
@@ -2818,7 +2831,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -3500,7 +3513,7 @@
   <dimension ref="A1:DG2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3510,10 +3523,10 @@
   <sheetData>
     <row r="1" spans="1:111" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C1">
         <v>2012</v>
@@ -3850,331 +3863,331 @@
       <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2" s="1">
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0</v>
+      </c>
+      <c r="I2" s="2">
         <v>921087</v>
       </c>
-      <c r="J2" s="1">
+      <c r="J2" s="2">
         <v>1003399</v>
       </c>
-      <c r="K2" s="1">
+      <c r="K2" s="2">
         <v>1093067</v>
       </c>
-      <c r="L2" s="1">
+      <c r="L2" s="2">
         <v>1190748</v>
       </c>
-      <c r="M2" s="1">
+      <c r="M2" s="2">
         <v>1244927</v>
       </c>
-      <c r="N2" s="1">
+      <c r="N2" s="2">
         <v>1301571</v>
       </c>
-      <c r="O2" s="1">
+      <c r="O2" s="2">
         <v>1360792</v>
       </c>
-      <c r="P2" s="1">
+      <c r="P2" s="2">
         <v>1422708</v>
       </c>
-      <c r="Q2" s="1">
+      <c r="Q2" s="2">
         <v>1487442</v>
       </c>
-      <c r="R2" s="1">
+      <c r="R2" s="2">
         <v>1555120</v>
       </c>
-      <c r="S2" s="1">
+      <c r="S2" s="2">
         <v>1625878</v>
       </c>
-      <c r="T2" s="1">
+      <c r="T2" s="2">
         <v>1699856</v>
       </c>
-      <c r="U2" s="1">
+      <c r="U2" s="2">
         <v>1777199</v>
       </c>
-      <c r="V2" s="1">
+      <c r="V2" s="2">
         <v>1858062</v>
       </c>
-      <c r="W2" s="1">
+      <c r="W2" s="2">
         <v>1942603</v>
       </c>
-      <c r="X2" s="1">
+      <c r="X2" s="2">
         <v>2030992</v>
       </c>
-      <c r="Y2" s="1">
+      <c r="Y2" s="2">
         <v>2123402</v>
       </c>
-      <c r="Z2" s="1">
+      <c r="Z2" s="2">
         <v>2220017</v>
       </c>
-      <c r="AA2" s="1">
+      <c r="AA2" s="2">
         <v>2321028</v>
       </c>
-      <c r="AB2" s="1">
+      <c r="AB2" s="2">
         <v>2426634</v>
       </c>
-      <c r="AC2" s="1">
+      <c r="AC2" s="2">
         <v>2537046</v>
       </c>
-      <c r="AD2" s="1">
+      <c r="AD2" s="2">
         <v>2652482</v>
       </c>
-      <c r="AE2" s="1">
+      <c r="AE2" s="2">
         <v>2773170</v>
       </c>
-      <c r="AF2" s="1">
+      <c r="AF2" s="2">
         <v>2899349</v>
       </c>
-      <c r="AG2" s="1">
+      <c r="AG2" s="2">
         <v>3031269</v>
       </c>
-      <c r="AH2" s="1">
+      <c r="AH2" s="2">
         <v>3169192</v>
       </c>
-      <c r="AI2" s="1">
+      <c r="AI2" s="2">
         <v>3313390</v>
       </c>
-      <c r="AJ2" s="1">
+      <c r="AJ2" s="2">
         <v>3464150</v>
       </c>
-      <c r="AK2" s="1">
+      <c r="AK2" s="2">
         <v>3621768</v>
       </c>
-      <c r="AL2" s="1">
+      <c r="AL2" s="2">
         <v>3786559</v>
       </c>
-      <c r="AM2" s="1">
+      <c r="AM2" s="2">
         <v>3958847</v>
       </c>
-      <c r="AN2" s="1">
+      <c r="AN2" s="2">
         <v>4057818</v>
       </c>
-      <c r="AO2" s="1">
+      <c r="AO2" s="2">
         <v>4159264</v>
       </c>
-      <c r="AP2" s="1">
+      <c r="AP2" s="2">
         <v>4263245</v>
       </c>
-      <c r="AQ2" s="1">
+      <c r="AQ2" s="2">
         <v>4369827</v>
       </c>
-      <c r="AR2" s="1">
+      <c r="AR2" s="2">
         <v>4479072</v>
       </c>
-      <c r="AS2" s="1">
+      <c r="AS2" s="2">
         <v>4591049</v>
       </c>
-      <c r="AT2" s="1">
+      <c r="AT2" s="2">
         <v>4705825</v>
       </c>
-      <c r="AU2" s="1">
+      <c r="AU2" s="2">
         <v>4823471</v>
       </c>
-      <c r="AV2" s="1">
+      <c r="AV2" s="2">
         <v>4944058</v>
       </c>
-      <c r="AW2" s="1">
+      <c r="AW2" s="2">
         <v>5067659</v>
       </c>
-      <c r="AX2" s="1">
+      <c r="AX2" s="2">
         <v>5194351</v>
       </c>
-      <c r="AY2" s="1">
+      <c r="AY2" s="2">
         <v>5324209</v>
       </c>
-      <c r="AZ2" s="1">
+      <c r="AZ2" s="2">
         <v>5457315</v>
       </c>
-      <c r="BA2" s="1">
+      <c r="BA2" s="2">
         <v>5593747</v>
       </c>
-      <c r="BB2" s="1">
+      <c r="BB2" s="2">
         <v>5733591</v>
       </c>
-      <c r="BC2" s="1">
+      <c r="BC2" s="2">
         <v>5876931</v>
       </c>
-      <c r="BD2" s="1">
+      <c r="BD2" s="2">
         <v>6023854</v>
       </c>
-      <c r="BE2" s="1">
+      <c r="BE2" s="2">
         <v>6174451</v>
       </c>
-      <c r="BF2" s="1">
+      <c r="BF2" s="2">
         <v>6328812</v>
       </c>
-      <c r="BG2" s="1">
+      <c r="BG2" s="2">
         <v>6487032</v>
       </c>
-      <c r="BH2" s="1">
+      <c r="BH2" s="2">
         <v>6649208</v>
       </c>
-      <c r="BI2" s="1">
+      <c r="BI2" s="2">
         <v>6815438</v>
       </c>
-      <c r="BJ2" s="1">
+      <c r="BJ2" s="2">
         <v>6985824</v>
       </c>
-      <c r="BK2" s="1">
+      <c r="BK2" s="2">
         <v>7160470</v>
       </c>
-      <c r="BL2" s="1">
+      <c r="BL2" s="2">
         <v>7339481</v>
       </c>
-      <c r="BM2" s="1">
+      <c r="BM2" s="2">
         <v>7522968</v>
       </c>
-      <c r="BN2" s="1">
+      <c r="BN2" s="2">
         <v>7711043</v>
       </c>
-      <c r="BO2" s="1">
+      <c r="BO2" s="2">
         <v>7903819</v>
       </c>
-      <c r="BP2" s="1">
+      <c r="BP2" s="2">
         <v>8101414</v>
       </c>
-      <c r="BQ2" s="1">
+      <c r="BQ2" s="2">
         <v>8303950</v>
       </c>
-      <c r="BR2" s="1">
+      <c r="BR2" s="2">
         <v>8511548</v>
       </c>
-      <c r="BS2" s="1">
+      <c r="BS2" s="2">
         <v>8724337</v>
       </c>
-      <c r="BT2" s="1">
+      <c r="BT2" s="2">
         <v>8942445</v>
       </c>
-      <c r="BU2" s="1">
+      <c r="BU2" s="2">
         <v>9166007</v>
       </c>
-      <c r="BV2" s="1">
+      <c r="BV2" s="2">
         <v>9395157</v>
       </c>
-      <c r="BW2" s="1">
+      <c r="BW2" s="2">
         <v>9630036</v>
       </c>
-      <c r="BX2" s="1">
+      <c r="BX2" s="2">
         <v>9870787</v>
       </c>
-      <c r="BY2" s="1">
+      <c r="BY2" s="2">
         <v>10117556</v>
       </c>
-      <c r="BZ2" s="1">
+      <c r="BZ2" s="2">
         <v>10370495</v>
       </c>
-      <c r="CA2" s="1">
+      <c r="CA2" s="2">
         <v>10629757</v>
       </c>
-      <c r="CB2" s="1">
+      <c r="CB2" s="2">
         <v>10895501</v>
       </c>
-      <c r="CC2" s="1">
+      <c r="CC2" s="2">
         <v>11167889</v>
       </c>
-      <c r="CD2" s="1">
+      <c r="CD2" s="2">
         <v>11447086</v>
       </c>
-      <c r="CE2" s="1">
+      <c r="CE2" s="2">
         <v>11733263</v>
       </c>
-      <c r="CF2" s="1">
+      <c r="CF2" s="2">
         <v>12026595</v>
       </c>
-      <c r="CG2" s="1">
+      <c r="CG2" s="2">
         <v>12327260</v>
       </c>
-      <c r="CH2" s="1">
+      <c r="CH2" s="2">
         <v>12635441</v>
       </c>
-      <c r="CI2" s="1">
+      <c r="CI2" s="2">
         <v>12951327</v>
       </c>
-      <c r="CJ2" s="1">
+      <c r="CJ2" s="2">
         <v>13275110</v>
       </c>
-      <c r="CK2" s="1">
+      <c r="CK2" s="2">
         <v>13606988</v>
       </c>
-      <c r="CL2" s="1">
+      <c r="CL2" s="2">
         <v>13947163</v>
       </c>
-      <c r="CM2" s="1">
+      <c r="CM2" s="2">
         <v>14295842</v>
       </c>
-      <c r="CN2" s="1">
+      <c r="CN2" s="2">
         <v>14653238</v>
       </c>
-      <c r="CO2" s="1">
+      <c r="CO2" s="2">
         <v>15019569</v>
       </c>
-      <c r="CP2" s="1">
+      <c r="CP2" s="2">
         <v>15395058</v>
       </c>
-      <c r="CQ2" s="1">
+      <c r="CQ2" s="2">
         <v>15779935</v>
       </c>
-      <c r="CR2" s="1">
+      <c r="CR2" s="2">
         <v>16174433</v>
       </c>
-      <c r="CS2" s="1">
+      <c r="CS2" s="2">
         <v>16578794</v>
       </c>
-      <c r="CT2" s="1">
+      <c r="CT2" s="2">
         <v>16993264</v>
       </c>
-      <c r="CU2" s="1">
+      <c r="CU2" s="2">
         <v>17418095</v>
       </c>
-      <c r="CV2" s="1">
+      <c r="CV2" s="2">
         <v>17853548</v>
       </c>
-      <c r="CW2" s="1">
+      <c r="CW2" s="2">
         <v>18299886</v>
       </c>
-      <c r="CX2" s="1">
+      <c r="CX2" s="2">
         <v>18757384</v>
       </c>
-      <c r="CY2" s="1">
+      <c r="CY2" s="2">
         <v>19226318</v>
       </c>
-      <c r="CZ2" s="1">
+      <c r="CZ2" s="2">
         <v>19706976</v>
       </c>
-      <c r="DA2" s="1">
+      <c r="DA2" s="2">
         <v>20199651</v>
       </c>
-      <c r="DB2" s="1">
+      <c r="DB2" s="2">
         <v>20704642</v>
       </c>
-      <c r="DC2" s="1">
+      <c r="DC2" s="2">
         <v>21222258</v>
       </c>
-      <c r="DD2" s="1">
+      <c r="DD2" s="2">
         <v>21752814</v>
       </c>
-      <c r="DE2" s="1">
+      <c r="DE2" s="2">
         <v>22296635</v>
       </c>
-      <c r="DF2" s="1">
+      <c r="DF2" s="2">
         <v>22854051</v>
       </c>
-      <c r="DG2" s="1">
+      <c r="DG2" s="2">
         <v>23425402</v>
       </c>
     </row>

</xml_diff>